<commit_message>
2024.11.30 - Save Final Output File
</commit_message>
<xml_diff>
--- a/Optimisation Output File.xlsx
+++ b/Optimisation Output File.xlsx
@@ -557,46 +557,46 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.54</v>
+        <v>0.46</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.35</v>
+        <v>0.29</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.54</v>
+        <v>0.49</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>0.35</v>
+        <v>0.27</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="3" ht="39" customHeight="1">
@@ -606,49 +606,49 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.64</v>
+        <v>0.55</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.68</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.63</v>
+        <v>0.57</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>0.63</v>
+        <v>0.58</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>0.36</v>
+        <v>0.3</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" ht="39" customHeight="1">
@@ -658,49 +658,49 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>0.45</v>
+        <v>0.36</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.51</v>
+        <v>0.44</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.48</v>
+        <v>0.41</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0.32</v>
+        <v>0.28</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.59</v>
+        <v>0.49</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="M4" s="1" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="O4" s="1" t="n">
         <v>0.35</v>
       </c>
-      <c r="N4" s="1" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>0.42</v>
-      </c>
       <c r="P4" s="1" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="5" ht="39" customHeight="1">
@@ -710,49 +710,49 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.45</v>
+        <v>0.36</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="P5" s="1" t="n">
         <v>0.42</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="N5" s="1" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="O5" s="1" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="P5" s="1" t="n">
-        <v>0.51</v>
       </c>
     </row>
     <row r="6" ht="39" customHeight="1">
@@ -762,49 +762,49 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.54</v>
+        <v>0.46</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0.64</v>
+        <v>0.55</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.51</v>
+        <v>0.44</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>0.42</v>
+        <v>0.33</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="M6" s="1" t="n">
         <v>0.42</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>0.46</v>
-      </c>
       <c r="N6" s="1" t="n">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="O6" s="1" t="n">
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="P6" s="1" t="n">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="7" ht="39" customHeight="1">
@@ -814,49 +814,49 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>0.35</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.42</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>0.28</v>
+        <v>0.24</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>0.33</v>
+        <v>0.29</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0.36</v>
+        <v>0.29</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>0.58</v>
+        <v>0.48</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>0.6</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="8" ht="39" customHeight="1">
@@ -866,22 +866,22 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.32</v>
+        <v>0.28</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>1</v>
@@ -890,25 +890,25 @@
         <v>-0</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>0.03</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="P8" s="1" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="9" ht="39" customHeight="1">
@@ -918,22 +918,22 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.45</v>
-      </c>
       <c r="E9" s="1" t="n">
-        <v>0.32</v>
+        <v>0.27</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>0.46</v>
+        <v>0.41</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.28</v>
+        <v>0.24</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>-0</v>
@@ -942,25 +942,25 @@
         <v>1</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>0.31</v>
+        <v>0.25</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>0.32</v>
+        <v>0.28</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="10" ht="39" customHeight="1">
@@ -970,49 +970,49 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0.68</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0.59</v>
+        <v>0.49</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>0.42</v>
+        <v>0.32</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>0.68</v>
+        <v>0.55</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>0.65</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="L10" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="O10" s="1" t="n">
         <v>0.34</v>
       </c>
-      <c r="M10" s="1" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="N10" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="O10" s="1" t="n">
-        <v>0.43</v>
-      </c>
       <c r="P10" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" ht="39" customHeight="1">
@@ -1022,46 +1022,46 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.54</v>
+        <v>0.49</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0.63</v>
+        <v>0.57</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>0.57</v>
+        <v>0.51</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.33</v>
+        <v>0.29</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.65</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="N11" s="1" t="n">
         <v>0.03</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>0.31</v>
+        <v>0.27</v>
       </c>
       <c r="P11" s="1" t="n">
         <v>0.01</v>
@@ -1074,34 +1074,34 @@
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.35</v>
+        <v>0.27</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>0.46</v>
+        <v>0.33</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>0.31</v>
+        <v>0.25</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.34</v>
+        <v>0.25</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>1</v>
@@ -1110,13 +1110,13 @@
         <v>-0.01</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="O12" s="1" t="n">
-        <v>0.42</v>
+        <v>0.31</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="13" ht="39" customHeight="1">
@@ -1126,34 +1126,34 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0.63</v>
+        <v>0.58</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>0.29</v>
+        <v>0.25</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>0.46</v>
+        <v>0.42</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0.03</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.51</v>
+        <v>0.45</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>-0.01</v>
@@ -1162,13 +1162,13 @@
         <v>1</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>0.33</v>
+        <v>0.29</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="14" ht="39" customHeight="1">
@@ -1178,49 +1178,49 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="D14" s="1" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="J14" s="1" t="n">
         <v>0.26</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>0.33</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>0.03</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="N14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="15" ht="39" customHeight="1">
@@ -1230,49 +1230,49 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="C15" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <v>0.36</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>0.44</v>
-      </c>
       <c r="G15" s="1" t="n">
-        <v>0.58</v>
+        <v>0.48</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>0.32</v>
+        <v>0.28</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.43</v>
+        <v>0.34</v>
       </c>
       <c r="K15" s="1" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="L15" s="1" t="n">
         <v>0.31</v>
       </c>
-      <c r="L15" s="1" t="n">
-        <v>0.42</v>
-      </c>
       <c r="M15" s="1" t="n">
-        <v>0.33</v>
+        <v>0.29</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.53</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="16" ht="39" customHeight="1">
@@ -1282,46 +1282,46 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>0.6</v>
+        <v>0.52</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="J16" s="1" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>0.53</v>
+        <v>0.44</v>
       </c>
       <c r="P16" s="1" t="n">
         <v>1</v>

</xml_diff>